<commit_message>
improved .tsv file keys
</commit_message>
<xml_diff>
--- a/Electrode names and scales matching.xlsx
+++ b/Electrode names and scales matching.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>electrode name</t>
+    <t>recording_scale</t>
   </si>
   <si>
-    <t>scale</t>
+    <t>electrode_name</t>
   </si>
 </sst>
 </file>
@@ -345,17 +345,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>